<commit_message>
update prefix, truncated function
update auto config & add prefix
draft truncated function
update template & enum
</commit_message>
<xml_diff>
--- a/public_html/template/Gen Entity Java Class Template.xlsx
+++ b/public_html/template/Gen Entity Java Class Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GenEntity" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="103">
   <si>
     <t>Primary Key</t>
   </si>
@@ -304,6 +304,36 @@
   </si>
   <si>
     <t>java.sql.Timestamp</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>dbl</t>
+  </si>
+  <si>
+    <t>sht</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>flt</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Truncated Num</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -365,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,6 +423,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +820,9 @@
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4"/>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
       <c r="J3" s="9"/>
       <c r="L3" t="s">
         <v>4</v>
@@ -818,7 +851,9 @@
       <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4"/>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
       <c r="J4" s="9"/>
       <c r="L4" t="s">
         <v>5</v>
@@ -847,7 +882,9 @@
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
       <c r="J5" s="9"/>
       <c r="L5" t="s">
         <v>6</v>
@@ -876,7 +913,9 @@
       <c r="H6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
       <c r="J6" s="9"/>
       <c r="L6" t="s">
         <v>48</v>
@@ -1699,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1750,7 @@
     <col min="2" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>52</v>
       </c>
@@ -1721,198 +1760,285 @@
       <c r="C1" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>56</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>87</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>79</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>85</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>66</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>85</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>59</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>60</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>68</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C25" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>